<commit_message>
change some info on xls file
</commit_message>
<xml_diff>
--- a/Schema_org/Structure_outil.xlsx
+++ b/Schema_org/Structure_outil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nouvellesdonnes.sharepoint.com/sites/NDOINTERNE/Documents partages/General/Capitalisation méthodologique/Projet Réseau/Projet digitalisation PU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FranckVIENOT\Downloads\Git\NDproject\UML\Schema_org\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="648" documentId="8_{56215971-E3CC-4ACE-9FD7-A949DBCF7786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE71CF86-C37C-48E8-AFCF-BEF34D714734}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543706BD-3DF7-4D9E-9FA6-6401BC38147F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{D6B886E7-0875-4E05-8A43-C45E22863F52}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{D6B886E7-0875-4E05-8A43-C45E22863F52}"/>
   </bookViews>
   <sheets>
     <sheet name="datas" sheetId="2" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="117">
   <si>
     <t>Champ</t>
   </si>
@@ -416,6 +416,21 @@
     <t>X: Non visible
 L: Lecture
 L+E: Lecture / Ecriture</t>
+  </si>
+  <si>
+    <t>Commentaire FVI</t>
+  </si>
+  <si>
+    <t>Clé étrangère en référence à la table collaborateur</t>
+  </si>
+  <si>
+    <t>Clé primaire</t>
+  </si>
+  <si>
+    <t>ID généré automatiquement lors de la création de la base</t>
+  </si>
+  <si>
+    <t>Libellé unique du type de contrat</t>
   </si>
 </sst>
 </file>
@@ -490,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,8 +530,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -650,13 +671,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -674,7 +695,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -683,52 +704,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -852,11 +828,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -873,59 +929,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -942,10 +984,22 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -954,18 +1008,53 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1286,13 +1375,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1303,7 +1392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1314,7 +1403,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1414,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1333,12 +1422,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1350,1938 +1439,2032 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83859F34-C32A-43E5-8596-5A05AF65EBF8}">
-  <dimension ref="A1:O92"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.54296875" customWidth="1"/>
-    <col min="6" max="6" width="78.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.54296875" customWidth="1"/>
-    <col min="8" max="8" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.26953125" customWidth="1"/>
-    <col min="10" max="14" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5546875" customWidth="1"/>
+    <col min="6" max="6" width="78.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="78.109375" customWidth="1"/>
+    <col min="8" max="8" width="3.5546875" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" customWidth="1"/>
+    <col min="11" max="15" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:16" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="G1" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="45"/>
-      <c r="H2" s="42" t="s">
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+    </row>
+    <row r="2" spans="1:16" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="61"/>
+      <c r="I2" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="J2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="K2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="L2" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="M2" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="N2" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="O2" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="P2" s="36" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="62"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="2"/>
+      <c r="C4" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="8"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
-      <c r="B5" s="19" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22" t="s">
+      <c r="C5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="4"/>
+      <c r="G5" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="9"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="19" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="39"/>
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="4"/>
+      <c r="C6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="64"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
-      <c r="B7" s="19" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="39"/>
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="4"/>
+      <c r="C7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="53"/>
+      <c r="G7" s="64"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="5"/>
-      <c r="O7" t="s">
+      <c r="N7" s="4"/>
+      <c r="O7" s="5"/>
+      <c r="P7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="39"/>
+      <c r="B8" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="4"/>
+      <c r="C8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="53"/>
+      <c r="G8" s="64"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="19" t="s">
+      <c r="N8" s="4"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="4"/>
+      <c r="C9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="53"/>
+      <c r="G9" s="64"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
-      <c r="B10" s="19" t="s">
+      <c r="N9" s="4"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="39"/>
+      <c r="B10" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="4"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="64"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" ht="22" x14ac:dyDescent="0.35">
-      <c r="A11" s="47"/>
-      <c r="B11" s="19" t="s">
+      <c r="N10" s="4"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="39"/>
+      <c r="B11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="4"/>
+      <c r="G11" s="65"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="47"/>
-      <c r="B12" s="24" t="s">
+      <c r="N11" s="4"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="39"/>
+      <c r="B12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="4"/>
+      <c r="G12" s="64"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="47"/>
-      <c r="B13" s="24" t="s">
+      <c r="N12" s="4"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="39"/>
+      <c r="B13" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="C13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="4"/>
+      <c r="G13" s="64"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="51"/>
-      <c r="B14" s="37" t="s">
+      <c r="N13" s="4"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="22" t="s">
+      <c r="C14" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="4"/>
+      <c r="G14" s="64"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="51"/>
-      <c r="B15" s="37" t="s">
+      <c r="N14" s="4"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="C15" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="4"/>
+      <c r="G15" s="64"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="48"/>
-      <c r="B16" s="25" t="s">
+      <c r="N15" s="4"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="41"/>
+      <c r="B16" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="29" t="s">
+      <c r="C16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="66"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="52" t="s">
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="67"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="2"/>
+      <c r="C18" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="8"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
-      <c r="B19" s="19" t="s">
+      <c r="N18" s="2"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="43"/>
+      <c r="B19" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22" t="s">
+      <c r="C19" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="4"/>
+      <c r="G19" s="64"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
-      <c r="B20" s="19" t="s">
+      <c r="N19" s="4"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="43"/>
+      <c r="B20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="22"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="4"/>
+      <c r="C20" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="53"/>
+      <c r="G20" s="64"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="53"/>
-      <c r="B21" s="19" t="s">
+      <c r="N20" s="4"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="43"/>
+      <c r="B21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="22"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="4"/>
+      <c r="C21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="53"/>
+      <c r="G21" s="64"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="53"/>
-      <c r="B22" s="19" t="s">
+      <c r="N21" s="4"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="43"/>
+      <c r="B22" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="22"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="4"/>
+      <c r="C22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="53"/>
+      <c r="G22" s="64"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="5"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
-      <c r="B23" s="19" t="s">
+      <c r="N22" s="4"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="22"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="4"/>
+      <c r="C23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="53"/>
+      <c r="G23" s="64"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="5"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="53"/>
-      <c r="B24" s="19" t="s">
+      <c r="N23" s="4"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="43"/>
+      <c r="B24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="C24" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="4"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="64"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="5"/>
-    </row>
-    <row r="25" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="19" t="s">
+      <c r="N24" s="4"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="43"/>
+      <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F25" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="4"/>
+      <c r="G25" s="65"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="5"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="53"/>
-      <c r="B26" s="19" t="s">
+      <c r="N25" s="4"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="23"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="4"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="54"/>
+      <c r="G26" s="65"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="5"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="53"/>
-      <c r="B27" s="24" t="s">
+      <c r="N26" s="4"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="20" t="s">
+      <c r="C27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="4"/>
+      <c r="G27" s="64"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="5"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="53"/>
-      <c r="B28" s="24" t="s">
+      <c r="N27" s="4"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="43"/>
+      <c r="B28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="22" t="s">
+      <c r="C28" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="4"/>
+      <c r="G28" s="64"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="5"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="53"/>
-      <c r="B29" s="37" t="s">
+      <c r="N28" s="4"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="22" t="s">
+      <c r="C29" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="4"/>
+      <c r="G29" s="64"/>
+      <c r="I29" s="9"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="5"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="53"/>
-      <c r="B30" s="37" t="s">
+      <c r="N29" s="4"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="43"/>
+      <c r="B30" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="22" t="s">
+      <c r="C30" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="4"/>
+      <c r="G30" s="64"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="5"/>
-    </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="54"/>
-      <c r="B31" s="25" t="s">
+      <c r="N30" s="4"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="44"/>
+      <c r="B31" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="29" t="s">
+      <c r="C31" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="6"/>
+      <c r="G31" s="66"/>
+      <c r="I31" s="10"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="7"/>
-    </row>
-    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="52" t="s">
+      <c r="N31" s="6"/>
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="67"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="18"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="2"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" s="8"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="53"/>
-      <c r="B34" s="32" t="s">
+      <c r="N33" s="2"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="22"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="4"/>
+      <c r="C34" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="53"/>
+      <c r="G34" s="64"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="5"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="53"/>
-      <c r="B35" s="32" t="s">
+      <c r="N34" s="4"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="43"/>
+      <c r="B35" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="22"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="4"/>
+      <c r="C35" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="53"/>
+      <c r="G35" s="64"/>
+      <c r="I35" s="9"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
-      <c r="N35" s="5"/>
-    </row>
-    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="54"/>
-      <c r="B36" s="33" t="s">
+      <c r="N35" s="4"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="44"/>
+      <c r="B36" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="29"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="6"/>
+      <c r="D36" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="55"/>
+      <c r="G36" s="66"/>
+      <c r="I36" s="10"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
-      <c r="N36" s="7"/>
-    </row>
-    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" s="52" t="s">
+      <c r="N36" s="6"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="67"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="2"/>
+      <c r="C38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="68"/>
+      <c r="I38" s="8"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="54"/>
-      <c r="B39" s="33" t="s">
+      <c r="N38" s="2"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="44"/>
+      <c r="B39" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="29"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="6"/>
+      <c r="D39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="55"/>
+      <c r="G39" s="66"/>
+      <c r="I39" s="10"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" s="7"/>
-    </row>
-    <row r="40" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A41" s="46" t="s">
+      <c r="N39" s="6"/>
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="67"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="18" t="s">
+      <c r="C41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="2"/>
+      <c r="G41" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="I41" s="8"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
-      <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="19" t="s">
+      <c r="N41" s="2"/>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="39"/>
+      <c r="B42" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="22" t="s">
+      <c r="C42" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="4"/>
+      <c r="G42" s="64"/>
+      <c r="I42" s="9"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="5"/>
-    </row>
-    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="26" t="s">
+      <c r="N42" s="4"/>
+      <c r="O42" s="5"/>
+    </row>
+    <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="41"/>
+      <c r="B43" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="29" t="s">
+      <c r="D43" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="6"/>
+      <c r="G43" s="66"/>
+      <c r="I43" s="10"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
-      <c r="N43" s="7"/>
-    </row>
-    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A45" s="46" t="s">
+      <c r="N43" s="6"/>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="67"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="18" t="s">
+      <c r="C45" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="H45" s="8"/>
-      <c r="I45" s="2"/>
+      <c r="G45" s="68"/>
+      <c r="I45" s="8"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
-      <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="48"/>
-      <c r="B46" s="26" t="s">
+      <c r="N45" s="2"/>
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="41"/>
+      <c r="B46" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="29" t="s">
+      <c r="C46" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="H46" s="10"/>
-      <c r="I46" s="6"/>
+      <c r="G46" s="66"/>
+      <c r="I46" s="10"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
-      <c r="N46" s="7"/>
-    </row>
-    <row r="47" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="14"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A48" s="46" t="s">
+      <c r="N46" s="6"/>
+      <c r="O46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="67"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="18" t="s">
+      <c r="C48" s="14"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="H48" s="8"/>
-      <c r="I48" s="2"/>
+      <c r="G48" s="68"/>
+      <c r="I48" s="8"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="3"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" s="47"/>
-      <c r="B49" s="19" t="s">
+      <c r="N48" s="2"/>
+      <c r="O48" s="3"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="39"/>
+      <c r="B49" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="22" t="s">
+      <c r="D49" s="18"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="4"/>
+      <c r="G49" s="64"/>
+      <c r="I49" s="9"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
-      <c r="N49" s="5"/>
-    </row>
-    <row r="50" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="48"/>
-      <c r="B50" s="26" t="s">
+      <c r="N49" s="4"/>
+      <c r="O49" s="5"/>
+    </row>
+    <row r="50" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="41"/>
+      <c r="B50" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="29" t="s">
+      <c r="D50" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H50" s="10"/>
-      <c r="I50" s="6"/>
+      <c r="G50" s="66"/>
+      <c r="I50" s="10"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
-      <c r="N50" s="7"/>
-    </row>
-    <row r="51" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" s="46" t="s">
+      <c r="N50" s="6"/>
+      <c r="O50" s="7"/>
+    </row>
+    <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="67"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="41" t="s">
+      <c r="F52" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="H52" s="8"/>
-      <c r="I52" s="2"/>
+      <c r="G52" s="69"/>
+      <c r="I52" s="8"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
-      <c r="N52" s="3"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="19" t="s">
+      <c r="N52" s="2"/>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" s="39"/>
+      <c r="B53" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="20" t="s">
+      <c r="C53" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E53" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="23" t="s">
+      <c r="F53" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="H53" s="9"/>
-      <c r="I53" s="4"/>
+      <c r="G53" s="65"/>
+      <c r="I53" s="9"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
-      <c r="N53" s="5"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="19" t="s">
+      <c r="N53" s="4"/>
+      <c r="O53" s="5"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" s="39"/>
+      <c r="B54" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="23" t="s">
+      <c r="C54" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="H54" s="9"/>
-      <c r="I54" s="4"/>
+      <c r="G54" s="65"/>
+      <c r="I54" s="9"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
-      <c r="N54" s="5"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="34" t="s">
+      <c r="N54" s="4"/>
+      <c r="O54" s="5"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" s="39"/>
+      <c r="B55" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F55" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="H55" s="9"/>
-      <c r="I55" s="4"/>
+      <c r="G55" s="64"/>
+      <c r="I55" s="9"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
-      <c r="N55" s="5"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A56" s="47"/>
-      <c r="B56" s="34" t="s">
+      <c r="N55" s="4"/>
+      <c r="O55" s="5"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56" s="39"/>
+      <c r="B56" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="22"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="4"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="64"/>
+      <c r="I56" s="9"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
-      <c r="N56" s="5"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A57" s="47"/>
-      <c r="B57" s="34" t="s">
+      <c r="N56" s="4"/>
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57" s="39"/>
+      <c r="B57" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="22"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="4"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="64"/>
+      <c r="I57" s="9"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
-      <c r="N57" s="5"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A58" s="47"/>
-      <c r="B58" s="34" t="s">
+      <c r="N57" s="4"/>
+      <c r="O57" s="5"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58" s="39"/>
+      <c r="B58" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="22"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="4"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="64"/>
+      <c r="I58" s="9"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
-      <c r="N58" s="5"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A59" s="47"/>
-      <c r="B59" s="34" t="s">
+      <c r="N58" s="4"/>
+      <c r="O58" s="5"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59" s="39"/>
+      <c r="B59" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="22"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="4"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="64"/>
+      <c r="I59" s="9"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
-      <c r="N59" s="5"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A60" s="47"/>
-      <c r="B60" s="34" t="s">
+      <c r="N59" s="4"/>
+      <c r="O59" s="5"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60" s="39"/>
+      <c r="B60" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="22"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="4"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="64"/>
+      <c r="I60" s="9"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
-      <c r="N60" s="5"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" s="47"/>
-      <c r="B61" s="34" t="s">
+      <c r="N60" s="4"/>
+      <c r="O60" s="5"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61" s="39"/>
+      <c r="B61" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="22"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="4"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="64"/>
+      <c r="I61" s="9"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
-      <c r="N61" s="5"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A62" s="47"/>
-      <c r="B62" s="34" t="s">
+      <c r="N61" s="4"/>
+      <c r="O61" s="5"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="39"/>
+      <c r="B62" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="23"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="4"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="54"/>
+      <c r="G62" s="65"/>
+      <c r="I62" s="9"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
-      <c r="N62" s="5"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A63" s="47"/>
-      <c r="B63" s="34" t="s">
+      <c r="N62" s="4"/>
+      <c r="O62" s="5"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63" s="39"/>
+      <c r="B63" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="23"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="4"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="65"/>
+      <c r="I63" s="9"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
-      <c r="N63" s="5"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" s="47"/>
-      <c r="B64" s="34" t="s">
+      <c r="N63" s="4"/>
+      <c r="O63" s="5"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64" s="39"/>
+      <c r="B64" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="23" t="s">
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="H64" s="9"/>
-      <c r="I64" s="4"/>
+      <c r="G64" s="65"/>
+      <c r="I64" s="9"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
-      <c r="N64" s="5"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A65" s="47"/>
-      <c r="B65" s="34" t="s">
+      <c r="N64" s="4"/>
+      <c r="O64" s="5"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="39"/>
+      <c r="B65" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="23" t="s">
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="H65" s="9"/>
-      <c r="I65" s="4"/>
+      <c r="G65" s="65"/>
+      <c r="I65" s="9"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
-      <c r="N65" s="5"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A66" s="47"/>
-      <c r="B66" s="34" t="s">
+      <c r="N65" s="4"/>
+      <c r="O65" s="5"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="39"/>
+      <c r="B66" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="23" t="s">
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="H66" s="9"/>
-      <c r="I66" s="4"/>
+      <c r="G66" s="65"/>
+      <c r="I66" s="9"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
-      <c r="N66" s="5"/>
-    </row>
-    <row r="67" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="48"/>
-      <c r="B67" s="35" t="s">
+      <c r="N66" s="4"/>
+      <c r="O66" s="5"/>
+    </row>
+    <row r="67" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="41"/>
+      <c r="B67" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
-      <c r="F67" s="36" t="s">
+      <c r="F67" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="H67" s="10"/>
-      <c r="I67" s="6"/>
+      <c r="G67" s="70"/>
+      <c r="I67" s="10"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
-      <c r="N67" s="7"/>
-    </row>
-    <row r="68" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="14"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A69" s="46" t="s">
+      <c r="N67" s="6"/>
+      <c r="O67" s="7"/>
+    </row>
+    <row r="68" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="67"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C69" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" s="18" t="s">
+      <c r="C69" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="H69" s="8"/>
-      <c r="I69" s="2"/>
+      <c r="G69" s="68"/>
+      <c r="I69" s="8"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
-      <c r="N69" s="3"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A70" s="47"/>
-      <c r="B70" s="19" t="s">
+      <c r="N69" s="2"/>
+      <c r="O69" s="3"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70" s="39"/>
+      <c r="B70" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="22" t="s">
+      <c r="C70" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="H70" s="9"/>
-      <c r="I70" s="4"/>
+      <c r="G70" s="64"/>
+      <c r="I70" s="9"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
-      <c r="N70" s="5"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A71" s="47"/>
-      <c r="B71" s="19" t="s">
+      <c r="N70" s="4"/>
+      <c r="O70" s="5"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71" s="39"/>
+      <c r="B71" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="22" t="s">
+      <c r="C71" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="H71" s="9"/>
-      <c r="I71" s="4"/>
+      <c r="G71" s="64"/>
+      <c r="I71" s="9"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
-      <c r="N71" s="5"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A72" s="47"/>
-      <c r="B72" s="34" t="s">
+      <c r="N71" s="4"/>
+      <c r="O71" s="5"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="39"/>
+      <c r="B72" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="22"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="4"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="64"/>
+      <c r="I72" s="9"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
-      <c r="N72" s="5"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A73" s="47"/>
-      <c r="B73" s="34" t="s">
+      <c r="N72" s="4"/>
+      <c r="O72" s="5"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73" s="39"/>
+      <c r="B73" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="22"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="4"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="64"/>
+      <c r="I73" s="9"/>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
-      <c r="N73" s="5"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A74" s="47"/>
-      <c r="B74" s="34" t="s">
+      <c r="N73" s="4"/>
+      <c r="O73" s="5"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" s="39"/>
+      <c r="B74" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="22"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="4"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="53"/>
+      <c r="G74" s="64"/>
+      <c r="I74" s="9"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
-      <c r="N74" s="5"/>
-    </row>
-    <row r="75" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="48"/>
-      <c r="B75" s="35" t="s">
+      <c r="N74" s="4"/>
+      <c r="O74" s="5"/>
+    </row>
+    <row r="75" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="41"/>
+      <c r="B75" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C75" s="26" t="s">
+      <c r="C75" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
-      <c r="F75" s="13"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="6"/>
+      <c r="F75" s="59"/>
+      <c r="G75" s="71"/>
+      <c r="I75" s="10"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
-      <c r="N75" s="7"/>
-    </row>
-    <row r="76" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="14"/>
-    </row>
-    <row r="77" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A77" s="46" t="s">
+      <c r="N75" s="6"/>
+      <c r="O75" s="7"/>
+    </row>
+    <row r="76" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="67"/>
+    </row>
+    <row r="77" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="41" t="s">
+      <c r="C77" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="H77" s="8"/>
-      <c r="I77" s="2"/>
+      <c r="G77" s="69"/>
+      <c r="I77" s="8"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
-      <c r="N77" s="3"/>
-    </row>
-    <row r="78" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A78" s="47"/>
-      <c r="B78" s="19" t="s">
+      <c r="N77" s="2"/>
+      <c r="O77" s="3"/>
+    </row>
+    <row r="78" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="39"/>
+      <c r="B78" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E78" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="23" t="s">
+      <c r="C78" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="H78" s="9"/>
-      <c r="I78" s="4"/>
+      <c r="G78" s="65"/>
+      <c r="I78" s="9"/>
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
-      <c r="N78" s="5"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A79" s="47"/>
-      <c r="B79" s="19" t="s">
+      <c r="N78" s="4"/>
+      <c r="O78" s="5"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A79" s="39"/>
+      <c r="B79" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C79" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="22" t="s">
+      <c r="C79" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="H79" s="9"/>
-      <c r="I79" s="4"/>
+      <c r="G79" s="64"/>
+      <c r="I79" s="9"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
-      <c r="N79" s="5"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A80" s="47"/>
-      <c r="B80" s="34" t="s">
+      <c r="N79" s="4"/>
+      <c r="O79" s="5"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A80" s="39"/>
+      <c r="B80" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="22"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="4"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="53"/>
+      <c r="G80" s="64"/>
+      <c r="I80" s="9"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
-      <c r="N80" s="5"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A81" s="47"/>
-      <c r="B81" s="34" t="s">
+      <c r="N80" s="4"/>
+      <c r="O80" s="5"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A81" s="39"/>
+      <c r="B81" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="22"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="4"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="53"/>
+      <c r="G81" s="64"/>
+      <c r="I81" s="9"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
-      <c r="N81" s="5"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A82" s="47"/>
-      <c r="B82" s="34" t="s">
+      <c r="N81" s="4"/>
+      <c r="O81" s="5"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82" s="39"/>
+      <c r="B82" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="22"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="4"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="53"/>
+      <c r="G82" s="64"/>
+      <c r="I82" s="9"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
-      <c r="N82" s="5"/>
-    </row>
-    <row r="83" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="48"/>
-      <c r="B83" s="35" t="s">
+      <c r="N82" s="4"/>
+      <c r="O82" s="5"/>
+    </row>
+    <row r="83" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="41"/>
+      <c r="B83" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C83" s="26" t="s">
+      <c r="C83" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
-      <c r="F83" s="13"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="6"/>
+      <c r="F83" s="59"/>
+      <c r="G83" s="71"/>
+      <c r="I83" s="10"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
       <c r="M83" s="6"/>
-      <c r="N83" s="7"/>
-    </row>
-    <row r="84" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="14"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="14"/>
-    </row>
-    <row r="85" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A85" s="46" t="s">
+      <c r="N83" s="6"/>
+      <c r="O83" s="7"/>
+    </row>
+    <row r="84" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="67"/>
+    </row>
+    <row r="85" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C85" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="41" t="s">
+      <c r="C85" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="H85" s="8"/>
-      <c r="I85" s="2"/>
+      <c r="G85" s="69"/>
+      <c r="I85" s="8"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="3"/>
-    </row>
-    <row r="86" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A86" s="47"/>
-      <c r="B86" s="19" t="s">
+      <c r="N85" s="2"/>
+      <c r="O85" s="3"/>
+    </row>
+    <row r="86" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="39"/>
+      <c r="B86" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C86" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E86" s="20"/>
-      <c r="F86" s="23" t="s">
+      <c r="C86" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" s="18"/>
+      <c r="F86" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="H86" s="9"/>
-      <c r="I86" s="4"/>
+      <c r="G86" s="65"/>
+      <c r="I86" s="9"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
-      <c r="N86" s="5"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A87" s="47"/>
-      <c r="B87" s="19" t="s">
+      <c r="N86" s="4"/>
+      <c r="O86" s="5"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" s="39"/>
+      <c r="B87" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C87" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" s="19"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="22" t="s">
+      <c r="C87" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="H87" s="9"/>
-      <c r="I87" s="4"/>
+      <c r="G87" s="64"/>
+      <c r="I87" s="9"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
-      <c r="N87" s="5"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A88" s="47"/>
-      <c r="B88" s="34" t="s">
+      <c r="N87" s="4"/>
+      <c r="O87" s="5"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88" s="39"/>
+      <c r="B88" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="22"/>
-      <c r="H88" s="9"/>
-      <c r="I88" s="4"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="53"/>
+      <c r="G88" s="64"/>
+      <c r="I88" s="9"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
-      <c r="N88" s="5"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A89" s="47"/>
-      <c r="B89" s="34" t="s">
+      <c r="N88" s="4"/>
+      <c r="O88" s="5"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89" s="39"/>
+      <c r="B89" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="22"/>
-      <c r="H89" s="9"/>
-      <c r="I89" s="4"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="53"/>
+      <c r="G89" s="64"/>
+      <c r="I89" s="9"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
-      <c r="N89" s="5"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A90" s="47"/>
-      <c r="B90" s="34" t="s">
+      <c r="N89" s="4"/>
+      <c r="O89" s="5"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" s="39"/>
+      <c r="B90" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="22"/>
-      <c r="H90" s="9"/>
-      <c r="I90" s="4"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="53"/>
+      <c r="G90" s="64"/>
+      <c r="I90" s="9"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
-      <c r="N90" s="5"/>
-    </row>
-    <row r="91" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="48"/>
-      <c r="B91" s="35" t="s">
+      <c r="N90" s="4"/>
+      <c r="O90" s="5"/>
+    </row>
+    <row r="91" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="41"/>
+      <c r="B91" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="C91" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
-      <c r="F91" s="13"/>
-      <c r="H91" s="10"/>
-      <c r="I91" s="6"/>
+      <c r="F91" s="59"/>
+      <c r="G91" s="71"/>
+      <c r="I91" s="10"/>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
       <c r="L91" s="6"/>
       <c r="M91" s="6"/>
-      <c r="N91" s="7"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="7"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A4:A16"/>
-    <mergeCell ref="A18:A31"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="19">
     <mergeCell ref="A52:A67"/>
     <mergeCell ref="A69:A75"/>
     <mergeCell ref="A85:A91"/>
@@ -3289,6 +3472,18 @@
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A48:A50"/>
     <mergeCell ref="A45:A46"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A4:A16"/>
+    <mergeCell ref="A18:A31"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3317,7 +3512,7 @@
           <x14:formula1>
             <xm:f>datas!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:N91</xm:sqref>
+          <xm:sqref>I4:O91</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>